<commit_message>
Cards (desk) & blog img
</commit_message>
<xml_diff>
--- a/CarMaster.xlsx
+++ b/CarMaster.xlsx
@@ -165,13 +165,13 @@
     <t>VideoPopUp + adapt + PP</t>
   </si>
   <si>
-    <t>Paragraph + adapt + PP</t>
-  </si>
-  <si>
     <t>ContactUs + adapt + PP</t>
   </si>
   <si>
     <t>CarSlider + adapt + PP</t>
+  </si>
+  <si>
+    <t>CardWithIcon + adapt + PP</t>
   </si>
 </sst>
 </file>
@@ -578,8 +578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1170,7 +1170,7 @@
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="3"/>
       <c r="B38" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="5">
@@ -1185,7 +1185,7 @@
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="3"/>
       <c r="B39" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C39" s="3"/>
       <c r="D39" s="5">
@@ -1200,7 +1200,7 @@
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="3"/>
       <c r="B40" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C40" s="3"/>
       <c r="D40" s="5">

</xml_diff>